<commit_message>
Fixed normalisation of <> and #
</commit_message>
<xml_diff>
--- a/experiments/results/llm_eval.xlsx
+++ b/experiments/results/llm_eval.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\32472\Desktop\MaastrichtUni\Year3\ThesisSep\CodeDataFinal\nl2sparql-thesis\experiments\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C19DF8A-3723-4656-83A5-F5604B0F038C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABDAC96-2AE0-4383-BF10-2B3229B1AAE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1226,8 +1226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
primekgqa testingup to dicitonary written
</commit_message>
<xml_diff>
--- a/experiments/results/llm_eval.xlsx
+++ b/experiments/results/llm_eval.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\32472\Desktop\MaastrichtUni\Year3\ThesisSep\CodeDataFinal\nl2sparql-thesis\experiments\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABDAC96-2AE0-4383-BF10-2B3229B1AAE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4E046E-049F-4A59-92D8-6B00C2685418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="6420" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>query_id</t>
   </si>
@@ -902,6 +902,38 @@
     # Additional filter to ensure we're in the time-chf context
     FILTER (CONTAINS(STR(?studyDesignExecution), "time-chf") || 
             CONTAINS(STR(?studyDesign), "time-chf"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>Deepseek_error</t>
+  </si>
+  <si>
+    <t>PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX cdio: &lt;https://w3id.org/CDIO/&gt;
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX ns1: &lt;http://purl.obolibrary.org/obo/bfo.owl#&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
+SELECT DISTINCT ?study
+WHERE {
+  GRAPH &lt;https://w3id.org/CDIO/graph/studies&gt; {
+    ?study a obi:StudyDesignExecution .
+    ?study bfo:concretizes ?study_design .
+    ?study_design bfo:has_part ?protocol .
+    # Look for diabetes in study primary purpose
+    {
+      ?protocol bfo:has_part ?purpose_spec .
+      ?purpose_spec ?has_value ?purpose_value .
+      FILTER (CONTAINS(LCASE(STR(?purpose_value)), "diabetes"))
+    }
+    UNION
+    # Optionally look for diabetes in inclusion criteria
+    {
+      ?protocol bfo:has_part ?inclusion_spec .
+      ?inclusion_spec ?has_value ?inclusion_value .
+      FILTER (CONTAINS(LCASE(STR(?inclusion_value)), "diabetes"))
+    }
   }
 }</t>
   </si>
@@ -1224,10 +1256,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1241,9 +1273,10 @@
     <col min="9" max="9" width="24.26953125" customWidth="1"/>
     <col min="10" max="10" width="12.36328125" customWidth="1"/>
     <col min="11" max="11" width="31.90625" customWidth="1"/>
+    <col min="12" max="12" width="17.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1277,8 +1310,11 @@
       <c r="K1" t="s">
         <v>46</v>
       </c>
+      <c r="L1" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1312,8 +1348,11 @@
       <c r="K2" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="L2" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1348,7 +1387,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1383,7 +1422,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
9 queries added, cdio -> cmeo KG updated, git ignored embbedings.npy as it exceeds 100 mb
</commit_message>
<xml_diff>
--- a/experiments/results/llm_eval.xlsx
+++ b/experiments/results/llm_eval.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\32472\Desktop\MaastrichtUni\Year3\ThesisSep\CodeDataFinal\nl2sparql-thesis\experiments\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4E046E-049F-4A59-92D8-6B00C2685418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD1F5D6-CC11-4A8C-8F52-81D574585F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6420" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>query_id</t>
   </si>
@@ -282,66 +282,6 @@
     ?protocol bfo:is_part_of ?study_design .
     ?study_design bfo:is_concretized_by ?study_exec .
     FILTER(?study_exec = cdio:time-chf)
-  }
-}</t>
-  </si>
-  <si>
-    <t>PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
-PREFIX cdio: &lt;https://w3id.org/CDIO/&gt;
-PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-PREFIX ns1: &lt;http://purl.obolibrary.org/obo/bfo.owl#&gt;
-PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
-SELECT ?study 
-GRAPH &lt;https://w3id.org/CDIO/graph/studies&gt; {
-  ?study cdio:study_design_variable_specification ?variable_spec .
-  ?variable_spec ns1:has_part &lt;https://w3id.org/CDIO/time-chf/diabetes&gt; .
-}</t>
-  </si>
-  <si>
-    <t>PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
-PREFIX cdio: &lt;https://w3id.org/CDIO/&gt;
-PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-PREFIX ns1: &lt;http://purl.obolibrary.org/obo/bfo.owl#&gt;
-PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
-SELECT ?study 
-GRAPH &lt;https://w3id.org/CDIO/graph/studies&gt; {
-  ?study ?p ?o .
-  FILTER EXISTS {
-    ?study cdio:study_design_variable_specification ?variable .
-    ?variable ?p2 ?o2 .
-    FILTER CONTAINS(str(?variable), "coronary heart disease") || CONTAINS(str(?o2), "coronary heart disease")
-  }
-}</t>
-  </si>
-  <si>
-    <t>PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
-PREFIX cdio: &lt;https://w3id.org/CDIO/&gt;
-PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-PREFIX ns1: &lt;http://purl.obolibrary.org/obo/bfo.owl#&gt;
-PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
-SELECT (COUNT(DISTINCT ?variable) AS ?variableCount)
-GRAPH &lt;https://w3id.org/CDIO/graph/studies&gt; {
-  ?study_design_execution cdio:concretizes ?study_design .
-  ?study_design bfo:has_part ?protocol .
-  ?protocol bfo:has_part ?variable_specification .
-  ?variable_specification ns1:has_part ?variable .
-  FILTER( regex(str(?study_design), "time-chf") || regex(str(?protocol), "time-chf") || regex(str(?variable_specification), "time-chf") )
-}</t>
-  </si>
-  <si>
-    <t>PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
-PREFIX cdio: &lt;https://w3id.org/CDIO/&gt;
-PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
-SELECT (COUNT(*) AS ?count)
-WHERE {
-  GRAPH &lt;https://w3id.org/CDIO/graph/studies&gt; {
-    ?variable ?p ?o .
-    FILTER CONTAINS(LCASE(STR(?variable)), "drug")
   }
 }</t>
   </si>
@@ -621,127 +561,7 @@
     <t>Claude_Sonnet-4.5</t>
   </si>
   <si>
-    <t>MetaAI_Llama-4</t>
-  </si>
-  <si>
     <t>Gemini_2.5-Flash</t>
-  </si>
-  <si>
-    <t>GPT-5_thinking</t>
-  </si>
-  <si>
-    <t>PREFIX bfo: http://purl.obolibrary.org/obo/bfo.owl/
-PREFIX cdio: https://w3id.org/CDIO/
-PREFIX dc: http://purl.org/dc/elements/1.1/
-PREFIX ns1: http://purl.obolibrary.org/obo/bfo.owl#
-PREFIX obi: http://purl.obolibrary.org/obo/obi.owl/
-PREFIX xsd: http://www.w3.org/2001/XMLSchema#
-SELECT DISTINCT ?study ?title
-WHERE {
-GRAPH https://w3id.org/CDIO/graph/studies
- {
-?study ?rel https://w3id.org/CDIO/time-chf/study_design_execution
- .
-https://w3id.org/CDIO/time-chf/study_design_execution
- bfo:concretizes https://w3id.org/CDIO/time-chf/study_design
- .
-https://w3id.org/CDIO/time-chf/study_design
- bfo:has_part https://w3id.org/CDIO/time-chf/protocol
- .
-https://w3id.org/CDIO/time-chf/protocol
- bfo:has_part https://w3id.org/CDIO/time-chf/study_design_variable_specification
- .
-https://w3id.org/CDIO/time-chf/study_design_variable_specification
- ns1:has_part https://w3id.org/CDIO/time-chf/diabetes
- .
-OPTIONAL { ?study dc:title ?title }
-}
-}</t>
-  </si>
-  <si>
-    <t>PREFIX bfo: http://purl.obolibrary.org/obo/bfo.owl/
-PREFIX cdio: https://w3id.org/CDIO/
-PREFIX dc: http://purl.org/dc/elements/1.1/
-PREFIX ns1: http://purl.obolibrary.org/obo/bfo.owl#
-PREFIX obi: http://purl.obolibrary.org/obo/obi.owl/
-PREFIX xsd: http://www.w3.org/2001/XMLSchema#
-SELECT DISTINCT ?study ?title ?description
-WHERE {
-GRAPH https://w3id.org/CDIO/graph/studies
- {
-?study bfo:concretizes https://w3id.org/CDIO/time-chf/study_design
- .
-https://w3id.org/CDIO/time-chf/study_design
- bfo:has_part https://w3id.org/CDIO/time-chf/protocol
- .
-https://w3id.org/CDIO/time-chf/protocol
- bfo:has_part https://w3id.org/CDIO/time-chf/study_design_variable_specification
- .
-https://w3id.org/CDIO/time-chf/study_design_variable_specification
- ns1:has_part https://w3id.org/CDIO/time-chf/angina
- .
-OPTIONAL { ?study dc:title ?title . }
-OPTIONAL { ?study dc:description ?description . }
-}
-}</t>
-  </si>
-  <si>
-    <t>prefix bfo: http://purl.obolibrary.org/obo/bfo.owl/
-prefix cdio: https://w3id.org/CDIO/
-prefix dc: http://purl.org/dc/elements/1.1/
-prefix ns1: http://purl.obolibrary.org/obo/bfo.owl#
-prefix obi: http://purl.obolibrary.org/obo/obi.owl/
-prefix xsd: http://www.w3.org/2001/XMLSchema#
-SELECT (COUNT(DISTINCT ?var) AS ?count)
-WHERE {
-GRAPH https://w3id.org/CDIO/graph/studies
- {
-https://w3id.org/CDIO/time-chf/study_design_execution
- bfo:concretizes https://w3id.org/CDIO/time-chf/study_design
- .
-https://w3id.org/CDIO/time-chf/study_design
- bfo:has_part https://w3id.org/CDIO/time-chf/protocol
- .
-https://w3id.org/CDIO/time-chf/protocol
- bfo:has_part https://w3id.org/CDIO/time-chf/study_design_variable_specification
- .
-https://w3id.org/CDIO/time-chf/study_design_variable_specification
- ns1:has_part ?var .
-}
-}</t>
-  </si>
-  <si>
-    <t>PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
-PREFIX cdio: &lt;https://w3id.org/CDIO/&gt;
-PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-PREFIX ns1: &lt;http://purl.obolibrary.org/obo/bfo.owl#&gt;
-PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
-PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
-SELECT (COUNT(DISTINCT ?var) AS ?drugVariableCount)
-WHERE {
-  GRAPH &lt;https://w3id.org/CDIO/graph/studies&gt; {
-    ?study a cdio:Study ;
-           dc:identifier ?studyId .
-    FILTER(CONTAINS(LCASE(STR(?studyId)), "time-chf"))
-    ?var rdfs:label ?label .
-    {
-      ?var a cdio:Variable .
-    }
-    UNION
-    {
-      ?var a obi:OBI_0000011 .
-    }
-    {
-      ?var bfo:is_part_of ?study .
-    }
-    UNION
-    {
-      ?var ns1:is_part_of ?study .
-    }
-    FILTER(CONTAINS(LCASE(STR(?label)), "drug"))
-  }
-}</t>
   </si>
   <si>
     <t>Deepseek</t>
@@ -821,120 +641,6 @@
 ?participants_spec bfo:is_part_of ?protocol .
 ?variable cdio:is_variable_of ?study_design_execution .
 }
-}</t>
-  </si>
-  <si>
-    <t>Deepseek_DeepThink</t>
-  </si>
-  <si>
-    <t>PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
-PREFIX cdio: &lt;https://w3id.org/CDIO/&gt;
-PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-PREFIX ns1: &lt;http://purl.obolibrary.org/obo/bfo.owl#&gt;
-PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
-SELECT DISTINCT ?study
-WHERE {
-  GRAPH &lt;https://w3id.org/CDIO/graph/studies&gt; {
-    ?study bfo:concretizes ?study_design .
-    ?study_design bfo:has_part ?protocol .
-    ?protocol bfo:has_part ?study_design_variable_specification .
-    ?study_design_variable_specification ns1:has_part &lt;https://w3id.org/CDIO/time-chf/diabetes&gt; .
-  }
-}</t>
-  </si>
-  <si>
-    <t>PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
-PREFIX cdio: &lt;https://w3id.org/CDIO/&gt;
-PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-PREFIX ns1: &lt;http://purl.obolibrary.org/obo/bfo.owl#&gt;
-PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
-SELECT DISTINCT ?study WHERE {
-  GRAPH &lt;https://w3id.org/CDIO/graph/studies&gt; {
-    ?study bfo:concretizes ?study_design .
-    ?study_design bfo:has_part ?protocol .
-    ?protocol bfo:has_part ?variable_spec .
-    ?variable_spec ns1:has_part ?condition .
-    # Filter for coronary heart disease related conditions
-    FILTER (CONTAINS(LCASE(STR(?condition)), "coronary") || 
-            CONTAINS(LCASE(STR(?condition)), "heart") ||
-            CONTAINS(LCASE(STR(?condition)), "angina") ||
-            CONTAINS(LCASE(STR(?condition)), "chd"))
-  }
-}</t>
-  </si>
-  <si>
-    <t>prefix bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
-prefix cdio: &lt;https://w3id.org/CDIO/&gt;
-prefix dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-prefix ns1: &lt;http://purl.obolibrary.org/obo/bfo.owl#&gt;
-prefix obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-prefix xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
-SELECT (COUNT(DISTINCT ?variable) AS ?variableCount)
-WHERE {
-  GRAPH &lt;https://w3id.org/CDIO/graph/studies&gt; {
-    &lt;https://w3id.org/CDIO/time-chf/study_design_execution&gt; bfo:concretizes &lt;https://w3id.org/CDIO/time-chf/study_design&gt; .
-    &lt;https://w3id.org/CDIO/time-chf/study_design&gt; bfo:has_part &lt;https://w3id.org/CDIO/time-chf/protocol&gt; .
-    &lt;https://w3id.org/CDIO/time-chf/protocol&gt; bfo:has_part &lt;https://w3id.org/CDIO/time-chf/study_design_variable_specification&gt; .
-    &lt;https://w3id.org/CDIO/time-chf/study_design_variable_specification&gt; ns1:has_part ?variable .
-  }
-}</t>
-  </si>
-  <si>
-    <t>PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
-PREFIX cdio: &lt;https://w3id.org/CDIO/&gt;
-PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-PREFIX ns1: &lt;http://purl.obolibrary.org/obo/bfo.owl#&gt;
-PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
-SELECT (COUNT(DISTINCT ?variable) AS ?count)
-WHERE {
-  GRAPH &lt;https://w3id.org/CDIO/graph/studies&gt; {
-    # Start with study design execution and follow the path to protocol
-    ?studyDesignExecution bfo:concretizes ?studyDesign .
-    ?studyDesign bfo:has_part ?protocol .
-    # Find drug-related variables that are part of the protocol
-    ?protocol bfo:has_part ?variable .
-    # Filter for drug-related variables (assuming they contain "drug" in their ID or label)
-    FILTER (CONTAINS(LCASE(STR(?variable)), "drug") || 
-            EXISTS { ?variable dc:title ?title . FILTER(CONTAINS(LCASE(?title), "drug")) })
-    # Additional filter to ensure we're in the time-chf context
-    FILTER (CONTAINS(STR(?studyDesignExecution), "time-chf") || 
-            CONTAINS(STR(?studyDesign), "time-chf"))
-  }
-}</t>
-  </si>
-  <si>
-    <t>Deepseek_error</t>
-  </si>
-  <si>
-    <t>PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
-PREFIX cdio: &lt;https://w3id.org/CDIO/&gt;
-PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-PREFIX ns1: &lt;http://purl.obolibrary.org/obo/bfo.owl#&gt;
-PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
-SELECT DISTINCT ?study
-WHERE {
-  GRAPH &lt;https://w3id.org/CDIO/graph/studies&gt; {
-    ?study a obi:StudyDesignExecution .
-    ?study bfo:concretizes ?study_design .
-    ?study_design bfo:has_part ?protocol .
-    # Look for diabetes in study primary purpose
-    {
-      ?protocol bfo:has_part ?purpose_spec .
-      ?purpose_spec ?has_value ?purpose_value .
-      FILTER (CONTAINS(LCASE(STR(?purpose_value)), "diabetes"))
-    }
-    UNION
-    # Optionally look for diabetes in inclusion criteria
-    {
-      ?protocol bfo:has_part ?inclusion_spec .
-      ?inclusion_spec ?has_value ?inclusion_value .
-      FILTER (CONTAINS(LCASE(STR(?inclusion_value)), "diabetes"))
-    }
-  }
 }</t>
   </si>
 </sst>
@@ -1256,27 +962,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="29.36328125" customWidth="1"/>
     <col min="3" max="3" width="17.36328125" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.36328125" customWidth="1"/>
     <col min="6" max="6" width="17.6328125" customWidth="1"/>
     <col min="7" max="7" width="27.7265625" customWidth="1"/>
     <col min="8" max="8" width="17.453125" customWidth="1"/>
-    <col min="9" max="9" width="24.26953125" customWidth="1"/>
-    <col min="10" max="10" width="12.36328125" customWidth="1"/>
-    <col min="11" max="11" width="31.90625" customWidth="1"/>
-    <col min="12" max="12" width="17.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1284,37 +986,25 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1328,31 +1018,19 @@
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>52</v>
-      </c>
     </row>
-    <row r="3" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1366,28 +1044,19 @@
         <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>48</v>
-      </c>
     </row>
-    <row r="4" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1401,28 +1070,19 @@
         <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>49</v>
-      </c>
     </row>
-    <row r="5" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1436,25 +1096,16 @@
         <v>14</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
only_schema and with_terms experiments 0-8 finished
</commit_message>
<xml_diff>
--- a/experiments/results/llm_eval.xlsx
+++ b/experiments/results/llm_eval.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\32472\Desktop\MaastrichtUni\Year3\ThesisSep\CodeDataFinal\nl2sparql-thesis\experiments\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4240080-AEED-428C-8211-7C5A4130748C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2EB6E2D-7FC0-447F-93F5-DA67F5792EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5050" yWindow="2170" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3380" yWindow="3380" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>query_id</t>
   </si>
@@ -39,11 +39,21 @@
     <t>Mistral_7B</t>
   </si>
   <si>
-    <t xml:space="preserve">PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
 PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX cmeo: &lt;https://w3id.org/CMEO/&gt;
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
-PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt; 
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
 SELECT DISTINCT ?study_name ?purpose ?inclusion
 WHERE {
     GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
@@ -66,15 +76,64 @@
            (BOUND(?inclusion) &amp;&amp; regex(lcase(str(?inclusion)), 'diabetes'))
          )
     }
-}
-</t>
-  </si>
-  <si>
-    <t>PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
 PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX cmeo: &lt;https://w3id.org/CMEO/&gt;
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
-PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt; 
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name ?purpose ?inclusion
+WHERE {
+    GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+         ?study a obi:study_design_execution ;
+                dc:identifier ?study_name;
+                ro:concretizes ?study_design.
+          ?study_design  ro:has_part ?protocol .
+         # Primary purpose specification
+         ?protocol ro:has_part ?purposeInst .
+         ?purposeInst a obi:objective_specification ;
+                      cmeo:has_value ?purpose .
+         # Inclusion criteria pattern (optional)
+         OPTIONAL {
+            ?protocol ro:has_part ?inclusionInst .
+            ?inclusionInst a obi:inclusion_criterion ;
+                           cmeo:has_value ?inclusion .
+         }
+         # Filter: Only include studies where the primary purpose or inclusion criteria contain "coronary heart disease"
+         FILTER( regex(lcase(str(?purpose)), 'coronary heart disease') ||
+           (BOUND(?inclusion) &amp;&amp; regex(lcase(str(?inclusion)), 'coronary heart disease'))
+         )
+    }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
 SELECT  (COUNT(?data_element) AS ?var_count)
 WHERE {
    GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
@@ -89,11 +148,21 @@
 }</t>
   </si>
   <si>
-    <t>PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
 PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX cmeo: &lt;https://w3id.org/CMEO/&gt;
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
-PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt; 
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
       SELECT  (COUNT(?data_element) AS ?var_count)
       WHERE {
         GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
@@ -115,135 +184,221 @@
       }</t>
   </si>
   <si>
-    <t xml:space="preserve">PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
 PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX cmeo: &lt;https://w3id.org/CMEO/&gt;
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
 PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
- GRAPH &lt;https://w3id.org/CDIO/graph/studies&gt; {
-SELECT ?study ?studyLabel WHERE {
-  ?study a &lt;https://w3id.org/CMEO/aachenhf/observational_design/protocol&gt;.
-  OPTIONAL {?study rdfs:label ?studyLabel.}
-  FILTER(STRSTARTS(str(?study), "diabetes"))
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT
+    ?study_name
+(GROUP_CONCAT(DISTINCT COALESCE(?part_uri); separator=";") AS ?all_parts_uri)
+(GROUP_CONCAT(DISTINCT COALESCE(?part_value); separator=";") AS ?all_parts_value)
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+      ?study  a cmeo:randomized_controlled_trial;
+      			ro:has_part   ?protocol;
+              dc:identifier ?study_name.
+      ?protocol a obi:protocol;
+              (ro:has_part)+ ?part_uri .
+      ?part_uri cmeo:has_value ?part_value.
+  }
+}
+GROUP BY ?study_name</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name ?description
+WHERE { 
+    GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+        ?study_design dc:identifier ?study_name;
+            iao:is_about ?descriptor;
+            ro:has_part ?prot .
+        ?descriptor rdfs:label ?description.
+        ?prot a obi:protocol;
+          ro:has_part ?obj_spec.
+        ?obj_spec a obi:objective_specification ;
+            cmeo:has_value ?obj_val.
+        ?prot ro:has_part ?ec.
+        ?ec a obi:eligibility_criterion;
+            ro:has_part ?inc.
+        ?inc a obi:inclusion_criterion;
+            ro:has_part ?spec_inc.
+        ?spec_inc  cmeo:has_value ?inc_value.
+    FILTER(contains  (?obj_val,"heart failure") || contains  (?inc_value,"heart failure"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT ?study_name (GROUP_CONCAT(DISTINCT LCASE(STR(?quality_value)); separator="; ") AS ?qualities)
+(GROUP_CONCAT(DISTINCT LCASE(STR(?quality_type)); separator="; ") AS ?quality_type)
+WHERE {
+GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+	 ?study_design dc:identifier ?study_name ;
+            ro:has_part ?prot .
+        ?prot a obi:protocol ;
+            ro:has_part ?ec .
+        ?ec a obi:eligibility_criterion ;
+            ro:is_concretized_by ?hse_uri .
+        ?hse_uri ro:has_output ?population .
+        ?population a obi:population ;
+            ro:has_characteristic ?quality .
+        OPTIONAL { ?quality rdfs:label ?characteristic_value }
+        OPTIONAL { ?quality a  ?characteristic_type }
 }
 }
-                         </t>
-  </si>
-  <si>
-    <t>PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+GROUP BY ?study_name
+LIMIT 3</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
 PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX cmeo: &lt;https://w3id.org/CMEO/&gt;
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
 PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
-SELECT DISTINCT ?study
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name 
+(GROUP_CONCAT(DISTINCT CONCAT(LCASE(STR(?diagnosis_value)), " [", STR(?min_val), "-", STR(?max_value), "]"); SEPARATOR="; ") AS ?population)
+(GROUP_CONCAT(DISTINCT LCASE(STR(?intervention_value)); separator="; ") AS ?interventions)
+(GROUP_CONCAT(DISTINCT LCASE(STR(?comparator_value)); separator="; ") AS ?comparators)
+(GROUP_CONCAT(DISTINCT LCASE(STR(?outcome_value)); separator="; ") AS ?outcomes)
+WHERE {  
+    GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+        ?study_design dc:identifier ?study_name;
+             ro:has_part ?prot .
+        ?prot a obi:protocol; 
+        # Population from inclusion criteria
+        	ro:has_part ?eligibility_criterion .
+        ?eligibility_criterion a obi:eligibility_criterion ;
+            ro:has_part ?inclusion_criteria .
+        ?inclusion_criteria a obi:inclusion_criterion ;
+            ro:has_part ?inc_part.
+    	#DIAGNOSTIC INCLUSION
+    	OPTIONAL{
+         ?inc_part a obi:health_status_inclusion_criterion;
+              cmeo:has_value ?diagnosis_value .
+         FILTER(contains  (?diagnosis_value, "nyha class ii"))
+      }
+      #AGE INCLUSION
+      OPTIONAL{
+         ?inc_part a obi:age_group_inclusion_criterion;
+            ro:has_part ?min_val_specification, ?max_value_specification.	
+          ?min_val_specification a obi:minimum_age_value_specification; 
+              cmeo:has_value ?min_val.
+          ?max_value_specification a obi:maximum_age_value_specification; 
+              cmeo:has_value  ?max_value.
+          FILTER(xsd:integer(?min_val) &gt;= 60 &amp;&amp; xsd:integer(?max_value) &lt;= 85)
+      }
+     # Intervention
+    	OPTIONAL{
+        ?prot ro:has_part ?intervention .
+        ?intervention a cmeo:intervention_specification; cmeo:has_value ?intervention_value .
+        FILTER(contains  (?intervention_value,"intensified"))
+     }
+        # Comparator
+        ?prot ro:has_part ?comparator .
+        ?comparator a cmeo:comparator_specification ;cmeo:has_value ?comparator_value .
+        FILTER(contains  (?comparator_value,"standard guided"))
+        # Outcomes
+     }
+      OPTIONAL{
+        ?prot ro:has_part ?outcome .
+        ?outcome a cmeo:outcome_specification ;
+                ro:has_part ?suboutcome_uri.
+        ?suboutcome_uri  cmeo:has_value ?outcome_value .
+        FILTER(contains  (?outcome_value,"survival"))
+    }
+}
+GROUP BY ?study_name</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT ?study_name
 WHERE {
   GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
-    ?study ro:has_part ?study_design_execution .
-    ?study_design_execution ro:concretizes ?observational_design .
-    ?observational_design ro:has_part ?protocol .
-    ?protocol ro:has_part ?variable_spec .
-    ?variable_spec ro:has_part cmeo:diabetes .
+    ?assignment a cmeo:data_use_permission_assignment ;
+                iao:is_about ?x_study ;
+                obi:has_specified_output ?data_policy ;
+                obi:has_specified_output ?data_modifier .
+    ?x_study a obi:study_design_execution ;
+             dc:identifier ?study_name .
+    ?data_policy a duo:data_use_permission ;
+                 rdfs:label "disease specific research"^^xsd:string ;
+                 iao:is_about ?disease_code .
+    ?data_modifier a duo:data_use_modifier ;
+                   rdfs:label "ethics approval required"^^xsd:string .
+    OPTIONAL { ?disease_code rdfs:label "congestive heart failure"^^xsd:string }
+    OPTIONAL { ?disease_code cmeo:has_value "42343007"^^xsd:string }
   }
-}</t>
-  </si>
-  <si>
-    <t>PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX cmeo: &lt;https://w3id.org/CMEO/&gt;
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
-PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
-SELECT (COUNT(?variable) AS ?variableCount)
-WHERE {
-  GRAPH&lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
-    cmeo:time-chf/ongoing 
-        &lt;http://purl.obolibrary.org/obo/iao.owl/is_about&gt; 
-        cmeo:time-chf/study_design_execution .
-    cmeo:time-chf/study_design_execution 
-        ro:concretizes 
-        cmeo:time-chf/randomized_controlled_trial .
-    cmeo:time-chf/randomized_controlled_trial 
-        ro:has_part 
-        cmeo:time-chf/randomized_controlled_trial/protocol .
-    cmeo:time-chf/randomized_controlled_trial/protocol 
-        ro:has_part 
-        cmeo:time-chf/study_design_variable_specification .
-    cmeo:time-chf/study_design_variable_specification 
-        ro:has_part 
-        ?variable .
-  }
-}</t>
-  </si>
-  <si>
-    <t>PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX cmeo: &lt;https://w3id.org/CMEO/&gt;
-PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
-SELECT (COUNT(DISTINCT ?variable) as ?count) WHERE {
-  GRAPH&lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
-    # Find the "hr" variable based on the last step in the RAG
-    ?trial a cmeo:RandomizedControlledTrial;
-             ro:has_part ?protocol .
-    ?protocol a cmeo:StudyDesignVariableSpecification;
-                ro:has_part ?variable.
-    FILTER(strstarts(str(?variable), str(cmeo:hr)))
-    # Follow the nhop_path defined in the RAG
-    OPTIONAL {
-      ?trial cmeo:is_about ?timeChfStudy .
-      ?timeChfStudy ro:concretizes ?studyDesignExecution .
-      ?studyDesignExecution cmeo:execution_phase ?ongoing .
-    }
-  }
-}</t>
-  </si>
-  <si>
-    <t>PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX cmeo: &lt;https://w3id.org/CMEO/&gt;
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
-PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
-SELECT (COUNT(?drugVar) AS ?drugVariableCount)
-WHERE {
-  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt;{
-    cmeo:time-chf/ongoing
-        &lt;http://purl.obolibrary.org/obo/iao.owl/is_about&gt; 
-        cmeo:time-chf/study_design_execution .
-    cmeo:time-chf/study_design_execution
-        ro:concretizes 
-        cmeo:time-chf/randomized_controlled_trial .
-    cmeo:time-chf/randomized_controlled_trial
-        ro:has_part 
-        cmeo:time-chf/randomized_controlled_trial/protocol .
-    cmeo:time-chf/randomized_controlled_trial/protocol
-        ro:has_part 
-        cmeo:time-chf/study_design_variable_specification .
-    cmeo:time-chf/study_design_variable_specification
-        ro:has_part 
-        ?drugVar .
-    ?drugVar dc:subject ?subject .
-    FILTER(CONTAINS(LCASE(STR(?subject)), "drug"))
-  }
-}</t>
-  </si>
-  <si>
-    <t>PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX cmeo: &lt;https://w3id.org/CMEO/&gt;
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
-PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
-SELECT (COUNT(DISTINCT ?variable) AS ?count) WHERE {
-  GRAPH&lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
-    # Start from the 'ongoing' context in the time-chf ontology
-    ?node1 cmeo:nhop_path* [ cmeo:nhop_path (cmeo:time-chf/ongoing ro:is_about
-cmeo:time-chf/study_design_execution) ] .
-    # Filter for study design variables with a drug or treatment relation
-    ?node1 cmeo:nhop_path* [ cmeo:nhop_path (cmeo:time-chf/study_design_execution ro:concretizes ?trial) ] .
-    ?trial ro:has_part+ ?treatmentVariable .
-    FILTER(contains(str(?treatmentVariable), "drug") || contains(str(?treatmentVariable), "treatment")) .
-    # Find the associated variable
-    ?treatmentVariable ro:has_part+ ?variable .
-  }
-}</t>
+}
+ORDER BY ?study_name</t>
+  </si>
+  <si>
+    <t>Claude</t>
+  </si>
+  <si>
+    <t>Llama</t>
   </si>
 </sst>
 </file>
@@ -564,20 +719,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="29.36328125" customWidth="1"/>
-    <col min="3" max="3" width="17.36328125" customWidth="1"/>
-    <col min="4" max="4" width="17.453125" customWidth="1"/>
+    <col min="3" max="5" width="17.36328125" customWidth="1"/>
+    <col min="6" max="6" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -588,55 +743,102 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B5" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
LLm evaluation experiments with all 9 queries and 4 models completed
</commit_message>
<xml_diff>
--- a/experiments/results/llm_eval.xlsx
+++ b/experiments/results/llm_eval.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\32472\Desktop\MaastrichtUni\Year3\ThesisSep\CodeDataFinal\nl2sparql-thesis\experiments\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2EB6E2D-7FC0-447F-93F5-DA67F5792EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F41C094-F3ED-423A-B94A-1447E2608730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3380" yWindow="3380" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>query_id</t>
   </si>
@@ -395,10 +395,1041 @@
 ORDER BY ?study_name</t>
   </si>
   <si>
-    <t>Claude</t>
-  </si>
-  <si>
-    <t>Llama</t>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study ?disease
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           iao:is_about ?descriptor .
+    ?descriptor cmeo:has_value ?disease .
+    FILTER(CONTAINS(LCASE(?disease), "diabetes"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study ?disease_label
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           iao:is_about ?descriptor .
+    ?descriptor cmeo:has_value ?disease_label .
+    FILTER(CONTAINS(LCASE(?disease_label), "coronary heart disease"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT (COUNT(?variable) AS ?variable_count)
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:study_design_variable_specification ;
+           dc:identifier ?id ;
+           ro:has_part ?variable .
+    FILTER(CONTAINS(LCASE(STR(?id)), "time-chf"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT (COUNT(?variable) AS ?drugVariableCount)
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:study_design_variable_specification ;
+           dc:identifier "time-chf"^^xsd:string ;
+           ro:has_part ?variable .
+    ?variable cmeo:has_value ?value .
+    FILTER(CONTAINS(LCASE(STR(?value)), "drug"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT ?trial ?protocol
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?trial a cmeo:randomized_controlled_trial ;
+           ro:has_part ?protocol .
+    ?protocol a obi:protocol .
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study ?study_label
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           iao:is_about ?descriptor ;
+           rdfs:label ?study_label .
+    ?descriptor cmeo:has_value ?condition_value .
+    FILTER(CONTAINS(LCASE(STR(?condition_value)), "heart failure"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT ?study ?populationCharacteristic ?value
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           ro:has_part ?eligibilityCriterion .
+    ?eligibilityCriterion a obi:eligibility_criterion ;
+           ro:has_part ?inclusionCriterion .
+    ?inclusionCriterion a obi:inclusion_criterion ;
+           ro:has_part ?populationCharacteristic .
+    ?populationCharacteristic cmeo:has_value ?value .
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study ?study_label
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           rdfs:label ?study_label ;
+           ro:has_part ?protocol .
+    ?protocol a obi:protocol ;
+              ro:has_part ?eligibility_criterion, ?intervention, ?comparator, ?outcome .
+    ?eligibility_criterion a obi:eligibility_criterion .
+    ?intervention a cmeo:intervention_specification .
+    ?comparator a cmeo:comparator_specification .
+    ?outcome a cmeo:outcome_specification .
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           iao:is_about ?descriptor ;
+           ro:has_part ?data_policy , ?data_modifier .
+    ?data_policy a duo:data_use_permission ;
+                 rdfs:label "disease specific research"^^xsd:string .
+    ?data_modifier a duo:data_use_modifier ;
+                   rdfs:label "ethics approval required"^^xsd:string .
+    ?descriptor cmeo:has_value ?disease .
+    FILTER(CONTAINS(LCASE(?disease), "congestive heart failure"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial, cmeo:observational_study.
+    ?study ro:is_about &lt;https://w3id.org/CMEO/disease/diabetes&gt;.
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+ SELECT ?study_identifier
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           dc:identifier ?study_identifier ;
+      rdfs:label ?study_name .
+    OPTIONAL {?study obi:is_about ?disease .}
+    FILTER (strstart(str(?disease), "coronary heart disease"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+ SELECT COUNT(DISTINCT ?variable) WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial .
+    ?study ro:has_part ?design .
+    ?design cmeo:has_value "time-chf"^^xsd:string .
+    ?design ro:part_of ?variable .
+    FILTER(strstarts(str(?variable), 'https://w3id.org/CMEO/'))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT (COUNT(DISTINCT ?drugVar) AS ?count) WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial, cmeo:clinical_study ;
+            cmeo:has_value ?studyType .
+    ?variable a cmeo:study_design_variable_specification ;
+              rdfs:label ?variableLabel ;
+              cmeo:has_value ?variableValue .
+    FILTER(STRSTARTS(str(?studyType), "drug"))
+    BIND(IF(langMatches(lang(?variableLabel), xsd:string, "en"), ?variableLabel,
+            ENCODE_FOR_RDF(translate(?variableLabel, " ", "_") as xsd:string)) as ?drugVar)
+    FILTER(STRSTARTS(str(?variableValue), "drug"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+ SELECT DISTINCT ?study WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial | ?study a obi:protocol ;
+              ro:has_part ?part .
+    FILTER(str(?part) KEEP BLANK() as xsd:string LIKE "%heart failure%"))}
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+ SELECT ?study ?age_group ?min_age ?max_age
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial|obi:observational_design ;
+             ro:part_of ?study_entity .
+    OPTIONAL {?study_entity obi:age_group_inclusion_criterion ?age_group_inclusion .}
+    OPTIONAL {?age_group_inclusion ro:has_part ?min_age_value_spec .}
+    OPTIONAL {?min_age_value_spec cmeo:has_value ?min_age .}
+    OPTIONAL {?age_group_inclusion ro:has_part ?max_age_value_spec .}
+    OPTIONAL {?max_age_value_spec cmeo:has_value ?max_age .}
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+ SELECT ?study WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           ro:has_part ?intervention ;
+           ro:has_part ?comparator ;
+           obi:objective_specification ?ob_objSpec ;
+           obcs:has_biological_context ?population ;
+           obi:eligibility_criterion ?inclusionCrit ;
+           obi:health_status_inclusion_criterion ?hsInclusionCrit .
+    FILTER(
+      langMatches(lang(?ob_objSpec), "en") &amp;&amp;
+      langMatches(lang(?population), "en") &amp;&amp;
+      langMatches(lang(?hsInclusionCrit), "en") &amp;&amp;
+      str(?inclusionCrit) = "chronic kidney disease on dialysis" &amp;&amp;
+      ?intervention cmeo:has_value ?picoIntervention &amp;&amp;
+      ?comparator cmeo:has_value ?picoComparator
+    )
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+ SELECT ?study_identifier
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial, cmeo:interventional_study ;
+           ro:is_concretized_by ?study_design ;
+           dc:identifier ?study_identifier .
+    FILTER(lang(?study_label, "en") = "congestive heart failure" ||
+           STRSTARTS(STR(?study_label), "congestive heart failure") ||
+           STR(?study_label) = "&lt;https://w3id.org/CMEO/biobank-eh/studies/
+congestive_heart_failure&gt;")
+    ?data_policy a duo:data_use_permission ;
+                rdfs:label "disease specific research"^^xsd:string ;
+    ?data_modifier a duo:data_use_modifier ;
+                   rdfs:label "ethics approval required"^^xsd:string .
+    OPTIONAL {
+      ?study ro:part_of ?criterion ;
+             cmeo:has_value ?health_status .
+      FILTER(STRSTARTS(STR(?health_status), "congestive heart failure"))
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?protocol
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?randomized_controlled_trial a cmeo:randomized_controlled_trial .
+    ?randomized_controlled_trial ro:has_part ?protocol .
+    ?protocol a obi:protocol .
+  }
+  FILTER(lang(label(?randomized_controlled_trial, und 'en'), und 'en') = "randomized_controlled_trial")
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt;
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt;
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study ?study_id
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           dc:identifier ?study_id .
+    ?study ro:has_part ?protocol .
+    ?protocol a obi:protocol ;
+              ro:has_part ?health_criterion .
+    ?health_criterion a obi:health_status_inclusion_criterion ;
+                      cmeo:has_value ?health_value .
+    FILTER(CONTAINS(LCASE(?health_value), "diabetes"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study ?identifier
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           dc:identifier ?identifier ;
+           iao:is_about ?descriptor .
+    ?descriptor cmeo:has_value ?description .
+    FILTER(CONTAINS(LCASE(?description), "coronary heart disease"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt;
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt;
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT (COUNT(?variable) AS ?count)
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           dc:identifier "time-chf"^^xsd:string .
+    ?study_design_variable a cmeo:study_design_variable_specification ;
+                          ro:has_part ?variable .
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT (COUNT(DISTINCT ?variable) AS ?count)
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           dc:identifier "time-chf"^^xsd:string ;
+           ro:has_part ?protocol .
+    ?protocol a obi:protocol ;
+              ro:has_part ?var_spec .
+    ?var_spec a cmeo:study_design_variable_specification ;
+              ro:has_part ?variable .
+    ?variable rdfs:label ?label .
+    FILTER(CONTAINS(LCASE(?label), "drug"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt;
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt;
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT ?rct ?protocol
+WHERE {
+    GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+        ?rct a cmeo:randomized_controlled_trial ;
+             ro:has_part ?protocol .
+        ?protocol a obi:protocol .
+    }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study ?studyId
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           dc:identifier ?studyId ;
+           ro:has_part ?protocol .
+    ?protocol a obi:protocol ;
+              ro:has_part ?inclusion .
+    ?inclusion a obi:inclusion_criterion ;
+               ro:has_part ?health_criterion .
+    ?health_criterion a obi:health_status_inclusion_criterion ;
+                      cmeo:has_value ?condition .
+    FILTER(REGEX(?condition, "heart failure", "i"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study ?study_id ?characteristic ?value
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           dc:identifier ?study_id ;
+           ro:has_part ?protocol .
+    ?protocol a obi:protocol ;
+              ro:has_part ?eligibility .
+    ?eligibility a obi:eligibility_criterion ;
+                 ro:has_part ?inclusion .
+    ?inclusion a obi:inclusion_criterion ;
+               ro:has_part ?characteristic .
+    ?characteristic cmeo:has_value ?value .
+  }
+}
+ORDER BY ?study_id</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt;
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt;
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study ?studyId
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           dc:identifier ?studyId ;
+           ro:has_part ?protocol .
+    ?protocol a obi:protocol ;
+              ro:has_part ?eligibility,
+                          ?outcome .
+    ?eligibility a obi:eligibility_criterion ;
+                 ro:has_part ?inclusion .
+    ?inclusion a obi:inclusion_criterion .
+    ?outcome a cmeo:outcome_specification .
+    OPTIONAL {
+      ?protocol ro:has_part ?intervention .
+      ?intervention a cmeo:intervention_specification .
+    }
+    OPTIONAL {
+      ?protocol ro:has_part ?comparator .
+      ?comparator a cmeo:comparator_specification .
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study ?study_id
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           dc:identifier ?study_id .
+    ?data_policy a duo:data_use_permission ;
+                 rdfs:label ?policy_label .
+    FILTER(CONTAINS(LCASE(?policy_label), "disease specific research"))
+    ?data_modifier a duo:data_use_modifier ;
+                   rdfs:label ?modifier_label .
+    FILTER(CONTAINS(LCASE(?modifier_label), "ethics approval required"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>Llama-3.1_8B</t>
+  </si>
+  <si>
+    <t>ClaudeSonnet-4.5</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt;
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt;
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT ?study
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt;
+  {
+    ?study a cmeo:randomized_controlled_trial ;
+           ro:has_part ?eligibility_criterion .
+    ?eligibility_criterion rdf:type obi:eligibility_criterion ;
+                            ro:has_part &lt;http://www.w3.org/2001/XMLSchema#string&gt;
+"congestive heart failure"^^xsd:string ;
+                            ro:part_of ?study_design .
+    ?data_policy rdfs:label "disease specific research"^^xsd:string .
+    ?eligibility_criterion2 rdf:type obi:eligibility_criterion ;
+                             ro:has_part
+&lt;http://www.w3.org/2001/XMLSchema#string&gt; "congestive heart failure"^^xsd:string
+;
+                             ro:part_of ?study_design .
+    ?data_policy2 rdfs:label "ethics approval required"^^xsd:string .
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT ?study
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+      ro:has_part ?outcome_specification .
+    ?outcome_specification a obi:objective_specification ;
+      cmeo:has_value ?disease_name .
+    FILTER ( STRDT(?disease_name, xsd:string) = "diabetes" )
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT ?study
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           ro:has_part ?outcome .
+    FILTER (cmeo:has_value(?outcome, "coronary heart disease")^^xsd:string)
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT (COUNT(DISTINCT ?variable) AS ?count)
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt;
+  {
+    ?study a cmeo:study_design .
+    ?variable ro:has_part ?study ;
+              rdfs:label ?label .
+    FILTER (regex(?label, "time-chf", "i"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT (COUNT(?var) AS ?count)
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           ro:has_part ?intervention .
+    ?intervention a cmeo:intervention_specification ;
+                  cmeo:has_value ?var .
+    FILTER regex(?var, "drug", "i")
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT ?protocol_specification ?has_part
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?randomized_controlled_trial a cmeo:randomized_controlled_trial ;
+                                 ro:has_part ?protocol_specification .
+    ?protocol_specification a obi:protocol ;
+                            ro:has_part ?has_part .
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT ?study
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt;
+    {
+      ?study a cmeo:randomized_controlled_trial ;
+             iao:is_about ?condition .
+      FILTER (regex(str(?condition), "heart failure"))
+    }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT ?study ?population_characteristic
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           obi:has_specified_input ?population_characteristic .
+    ?population_characteristic a obi:eligibility_criterion; 
+                                 obi:inclusion_criterion .
+                                 obi:exclusion_criterion .
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT ?study
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           ro:has_part a obi:inclusion_criterion ;
+                        ro:part_of ?eligibility  .
+    ?eligibility a obi:eligibility_criterion ;
+                 ro:has_part 
+                   a obi:health_status_inclusion_criterion ;
+                   cmeo:has_value ?criterion .
+  }
+}</t>
   </si>
 </sst>
 </file>
@@ -721,14 +1752,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="29.36328125" customWidth="1"/>
-    <col min="3" max="5" width="17.36328125" customWidth="1"/>
+    <col min="3" max="3" width="26.453125" customWidth="1"/>
+    <col min="4" max="5" width="17.36328125" customWidth="1"/>
     <col min="6" max="6" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -743,10 +1775,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -759,10 +1791,18 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3">
@@ -771,10 +1811,18 @@
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -783,10 +1831,18 @@
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -795,10 +1851,18 @@
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A6">
@@ -807,6 +1871,18 @@
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A7">
@@ -815,6 +1891,18 @@
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A8">
@@ -823,6 +1911,18 @@
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A9">
@@ -831,6 +1931,18 @@
       <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A10">
@@ -838,6 +1950,18 @@
       </c>
       <c r="B10" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>